<commit_message>
adding egg weight and adding footer to sidebar
</commit_message>
<xml_diff>
--- a/master_template.xlsx
+++ b/master_template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Weeks</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t xml:space="preserve">Egg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egg Weight</t>
   </si>
   <si>
     <t xml:space="preserve">Feed</t>
@@ -283,10 +286,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AJ11"/>
+  <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -300,7 +303,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="7.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="1" width="7.18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -320,6 +323,7 @@
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
@@ -358,18 +362,21 @@
       <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -385,6 +392,9 @@
         <v>0</v>
       </c>
       <c r="L3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -407,6 +417,9 @@
       <c r="L4" s="7" t="n">
         <v>0</v>
       </c>
+      <c r="M4" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
@@ -425,6 +438,9 @@
         <v>0</v>
       </c>
       <c r="L5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -441,7 +457,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="0"/>
+      <c r="M10" s="1"/>
       <c r="N10" s="0"/>
       <c r="O10" s="0"/>
       <c r="P10" s="0"/>
@@ -465,6 +481,7 @@
       <c r="AH10" s="0"/>
       <c r="AI10" s="0"/>
       <c r="AJ10" s="0"/>
+      <c r="AK10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J11" s="9"/>
@@ -472,7 +489,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>